<commit_message>
The 'TAWA_CustRequirements'document has been modified
</commit_message>
<xml_diff>
--- a/TAWA_CustRequirements.xlsx
+++ b/TAWA_CustRequirements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\PM project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\project management\project\Travel-Adviser-Web-Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,51 +24,175 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Travel Advisor web application</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>The holidays will be set from this web site. This application shall
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <r>
+      <t xml:space="preserve">Description: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The holidays will be set from this web site. This application shall
 provide a window for the different places and tours that a visitor
 can view before travelling to a specific country. This site should
-guide him/her through from the start to the end of the journey</t>
-  </si>
-  <si>
-    <t>Features</t>
-  </si>
-  <si>
-    <t>1. The user can register and login and land on a photo gallery of
-the top travel destination
-2. A platform for booking a flight should be provided so the user
-can easily explore different airlines and book his flight.
-3. A rating system will be provided so the visitor can send his 
-feedback and share his experience</t>
-  </si>
-  <si>
-    <t>Constrains</t>
-  </si>
-  <si>
-    <t>1- Web-based system / PC needed
-2- Unique user IDs
-3- Admin features needed</t>
-  </si>
-  <si>
-    <t>Stakeholder</t>
-  </si>
-  <si>
-    <t>1- User
-2- Admin</t>
+guide him/her through from the start to the end of the journey.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Project Name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Travel Advisor web application.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Author: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Esraa Salah.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Creation Date: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>27/4/2019.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Constrains:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1- Web-based system / PC needed.
+2- Unique user IDs.
+3- Admin features needed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Stakeholder:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1- User.
+2- Admin.</t>
+    </r>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>FEATURES</t>
+  </si>
+  <si>
+    <t>TAWA_CR_001</t>
+  </si>
+  <si>
+    <t>TAWA_CR_002</t>
+  </si>
+  <si>
+    <t>TAWA_CR_003</t>
+  </si>
+  <si>
+    <t>TAWA_CR_004</t>
+  </si>
+  <si>
+    <t>TAWA_CR_005</t>
+  </si>
+  <si>
+    <t>The user can register and login into the website.</t>
+  </si>
+  <si>
+    <t>A platform for booking a flight should be provided so the user can easily explore different airlines.</t>
+  </si>
+  <si>
+    <t>The user can book his flight.</t>
+  </si>
+  <si>
+    <t>The user will land on a photo gallery of the  top travel destination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A rating system will be provided so the visitor can send his feedback and share his experience.
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,16 +200,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -94,21 +244,144 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -390,123 +663,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A4" sqref="A4:T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="187.88671875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:21" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="18"/>
+    </row>
+    <row r="2" spans="1:21" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="18"/>
+    </row>
+    <row r="3" spans="1:21" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="18"/>
+    </row>
+    <row r="4" spans="1:21" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="15"/>
+    </row>
+    <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+    </row>
+    <row r="6" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A3:T3"/>
+    <mergeCell ref="A4:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>